<commit_message>
ekspor akademik berhasil sampai tabel 3
</commit_message>
<xml_diff>
--- a/common/required/kriteria9/apt/template/kuantitatif_akademik.xlsx
+++ b/common/required/kriteria9/apt/template/kuantitatif_akademik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adryanev\Code\php\kriteria\common\required\kriteria9\apt\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B34D3DD-B950-42E5-8303-D1A96A53CCEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D3FD9E-BDEB-4D2B-9F43-7551B99B5869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="839" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30405" yWindow="6930" windowWidth="15375" windowHeight="8085" tabRatio="839" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="14" r:id="rId1"/>
@@ -1194,7 +1194,7 @@
     <author>Suharyadi</author>
   </authors>
   <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000001000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1208,7 +1208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000002000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1222,7 +1222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000003000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -2487,7 +2487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="364">
   <si>
     <t>No.</t>
   </si>
@@ -4355,7 +4355,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4652,6 +4652,9 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4763,67 +4766,7 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color theme="0"/>
@@ -5288,62 +5231,62 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="101"/>
-      <c r="S3" s="101"/>
-      <c r="T3" s="101"/>
-      <c r="U3" s="101"/>
-      <c r="V3" s="101"/>
-      <c r="W3" s="101"/>
-      <c r="X3" s="101"/>
-      <c r="Y3" s="101"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="102"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -5373,33 +5316,33 @@
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="106" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="105"/>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="105"/>
-      <c r="S5" s="105"/>
-      <c r="T5" s="105"/>
-      <c r="U5" s="105"/>
-      <c r="V5" s="105"/>
-      <c r="W5" s="105"/>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="106"/>
+      <c r="T5" s="106"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="106"/>
+      <c r="X5" s="106"/>
+      <c r="Y5" s="106"/>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -5440,23 +5383,23 @@
       <c r="G7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="102"/>
-      <c r="N7" s="102"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="102"/>
-      <c r="R7" s="102"/>
-      <c r="S7" s="102"/>
-      <c r="T7" s="102"/>
-      <c r="U7" s="102"/>
-      <c r="V7" s="102"/>
-      <c r="W7" s="102"/>
-      <c r="X7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="103"/>
+      <c r="V7" s="103"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="103"/>
       <c r="Y7" s="11"/>
     </row>
     <row r="8" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5498,13 +5441,13 @@
       <c r="G9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -5697,15 +5640,15 @@
       <c r="G16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="103"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="103"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="103"/>
-      <c r="N16" s="103"/>
-      <c r="O16" s="103"/>
-      <c r="P16" s="103"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="104"/>
+      <c r="M16" s="104"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="104"/>
+      <c r="P16" s="104"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
@@ -5925,23 +5868,23 @@
       <c r="G24" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="103"/>
-      <c r="I24" s="103"/>
-      <c r="J24" s="103"/>
-      <c r="K24" s="103"/>
-      <c r="L24" s="103"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
-      <c r="U24" s="103"/>
-      <c r="V24" s="103"/>
-      <c r="W24" s="103"/>
-      <c r="X24" s="103"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="104"/>
+      <c r="V24" s="104"/>
+      <c r="W24" s="104"/>
+      <c r="X24" s="104"/>
       <c r="Y24" s="11"/>
     </row>
     <row r="25" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5979,23 +5922,23 @@
       <c r="E26" s="11"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="103"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="103"/>
-      <c r="K26" s="103"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="103"/>
-      <c r="N26" s="103"/>
-      <c r="O26" s="103"/>
-      <c r="P26" s="103"/>
-      <c r="Q26" s="103"/>
-      <c r="R26" s="103"/>
-      <c r="S26" s="103"/>
-      <c r="T26" s="103"/>
-      <c r="U26" s="103"/>
-      <c r="V26" s="103"/>
-      <c r="W26" s="103"/>
-      <c r="X26" s="103"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="104"/>
+      <c r="M26" s="104"/>
+      <c r="N26" s="104"/>
+      <c r="O26" s="104"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="104"/>
+      <c r="U26" s="104"/>
+      <c r="V26" s="104"/>
+      <c r="W26" s="104"/>
+      <c r="X26" s="104"/>
       <c r="Y26" s="11"/>
     </row>
     <row r="27" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6037,13 +5980,13 @@
       <c r="G28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="103"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
-      <c r="K28" s="103"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
-      <c r="N28" s="103"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="104"/>
+      <c r="N28" s="104"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="13"/>
@@ -6095,16 +6038,16 @@
       <c r="G30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="103"/>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="103"/>
-      <c r="L30" s="103"/>
-      <c r="M30" s="103"/>
-      <c r="N30" s="103"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="104"/>
+      <c r="L30" s="104"/>
+      <c r="M30" s="104"/>
+      <c r="N30" s="104"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
@@ -6153,15 +6096,15 @@
       <c r="G32" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="103"/>
-      <c r="I32" s="103"/>
-      <c r="J32" s="103"/>
-      <c r="K32" s="103"/>
-      <c r="L32" s="103"/>
-      <c r="M32" s="103"/>
-      <c r="N32" s="103"/>
-      <c r="O32" s="103"/>
-      <c r="P32" s="103"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="104"/>
+      <c r="N32" s="104"/>
+      <c r="O32" s="104"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
       <c r="S32" s="13"/>
@@ -6211,15 +6154,15 @@
       <c r="G34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="103"/>
-      <c r="I34" s="103"/>
-      <c r="J34" s="103"/>
-      <c r="K34" s="103"/>
-      <c r="L34" s="103"/>
-      <c r="M34" s="103"/>
-      <c r="N34" s="103"/>
-      <c r="O34" s="103"/>
-      <c r="P34" s="103"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
+      <c r="L34" s="104"/>
+      <c r="M34" s="104"/>
+      <c r="N34" s="104"/>
+      <c r="O34" s="104"/>
+      <c r="P34" s="104"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
@@ -6269,11 +6212,11 @@
       <c r="G36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H36" s="103"/>
-      <c r="I36" s="103"/>
-      <c r="J36" s="103"/>
-      <c r="K36" s="103"/>
-      <c r="L36" s="103"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="104"/>
+      <c r="J36" s="104"/>
+      <c r="K36" s="104"/>
+      <c r="L36" s="104"/>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
@@ -6385,15 +6328,15 @@
       <c r="G40" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="103"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="103"/>
-      <c r="K40" s="103"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-      <c r="N40" s="103"/>
-      <c r="O40" s="103"/>
-      <c r="P40" s="103"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
+      <c r="L40" s="104"/>
+      <c r="M40" s="104"/>
+      <c r="N40" s="104"/>
+      <c r="O40" s="104"/>
+      <c r="P40" s="104"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
@@ -6572,12 +6515,12 @@
       <c r="R46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S46" s="103"/>
-      <c r="T46" s="103"/>
-      <c r="U46" s="103"/>
-      <c r="V46" s="103"/>
-      <c r="W46" s="103"/>
-      <c r="X46" s="103"/>
+      <c r="S46" s="104"/>
+      <c r="T46" s="104"/>
+      <c r="U46" s="104"/>
+      <c r="V46" s="104"/>
+      <c r="W46" s="104"/>
+      <c r="X46" s="104"/>
       <c r="Y46" s="11"/>
     </row>
     <row r="47" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6632,12 +6575,12 @@
       <c r="R48" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S48" s="104">
+      <c r="S48" s="105">
         <f ca="1">TODAY()</f>
-        <v>44198</v>
-      </c>
-      <c r="T48" s="104"/>
-      <c r="U48" s="104"/>
+        <v>44200</v>
+      </c>
+      <c r="T48" s="105"/>
+      <c r="U48" s="105"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
@@ -6754,7 +6697,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6775,24 +6718,24 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="115" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="116" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="116"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="30" t="s">
         <v>74</v>
       </c>
@@ -6802,7 +6745,7 @@
       <c r="E4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="117"/>
+      <c r="F4" s="118"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -6851,10 +6794,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="112"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="36">
         <f>SUM(C6:C7)</f>
         <v>0</v>
@@ -6899,7 +6842,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6920,28 +6863,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="117" t="s">
+      <c r="H3" s="118" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>86</v>
       </c>
@@ -6954,8 +6897,8 @@
       <c r="F4" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -7035,10 +6978,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="112"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7157,10 +7100,10 @@
       <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="112"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="34">
         <f>SUM(C5:C6)</f>
         <v>0</v>
@@ -7217,28 +7160,28 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="118" t="s">
+      <c r="A3" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118" t="s">
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="118" t="s">
+      <c r="H3" s="119" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="118"/>
-      <c r="B4" s="118"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="53" t="s">
         <v>86</v>
       </c>
@@ -7251,8 +7194,8 @@
       <c r="F4" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -7332,10 +7275,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="112"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7462,10 +7405,10 @@
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="112"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="36">
         <f>SUM(C5:C6)</f>
         <v>0</v>
@@ -7523,24 +7466,24 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="120" t="s">
+      <c r="A3" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="120" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119" t="s">
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
-      <c r="B4" s="121"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="26" t="s">
         <v>62</v>
       </c>
@@ -7550,7 +7493,7 @@
       <c r="E4" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="119"/>
+      <c r="F4" s="120"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
@@ -7618,10 +7561,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="112"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7687,24 +7630,24 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="120" t="s">
+      <c r="A3" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="120" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119" t="s">
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
-      <c r="B4" s="121"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="26" t="s">
         <v>62</v>
       </c>
@@ -7714,7 +7657,7 @@
       <c r="E4" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="119"/>
+      <c r="F4" s="120"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
@@ -7782,10 +7725,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="112"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7826,11 +7769,11 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7938,7 +7881,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="A29" sqref="A29:C29"/>
@@ -7967,28 +7910,28 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="118" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117" t="s">
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="30" t="s">
         <v>62</v>
       </c>
@@ -7998,7 +7941,7 @@
       <c r="F4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="117"/>
+      <c r="G4" s="118"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -8024,10 +7967,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="122">
+      <c r="A6" s="123">
         <v>1</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -8042,8 +7985,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="123"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="124"/>
       <c r="C7" s="20" t="s">
         <v>112</v>
       </c>
@@ -8056,8 +7999,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="123"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="20" t="s">
         <v>113</v>
       </c>
@@ -8070,11 +8013,11 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="112" t="s">
+      <c r="A9" s="123"/>
+      <c r="B9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="112"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="94">
         <f>SUM(D6:D8)</f>
         <v>0</v>
@@ -8093,10 +8036,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="122">
+      <c r="A10" s="123">
         <v>2</v>
       </c>
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="124" t="s">
         <v>114</v>
       </c>
       <c r="C10" s="20" t="s">
@@ -8111,8 +8054,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="123"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="124"/>
       <c r="C11" s="20" t="s">
         <v>115</v>
       </c>
@@ -8125,8 +8068,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="123"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="20" t="s">
         <v>116</v>
       </c>
@@ -8139,8 +8082,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
-      <c r="B13" s="123"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="20" t="s">
         <v>117</v>
       </c>
@@ -8153,8 +8096,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="122"/>
-      <c r="B14" s="123"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="20" t="s">
         <v>113</v>
       </c>
@@ -8167,11 +8110,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="122"/>
-      <c r="B15" s="112" t="s">
+      <c r="A15" s="123"/>
+      <c r="B15" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="112"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="94">
         <f>SUM(D10:D14)</f>
         <v>0</v>
@@ -8190,10 +8133,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="122">
+      <c r="A16" s="123">
         <v>3</v>
       </c>
-      <c r="B16" s="123" t="s">
+      <c r="B16" s="124" t="s">
         <v>129</v>
       </c>
       <c r="C16" s="20" t="s">
@@ -8208,8 +8151,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
-      <c r="B17" s="123"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="20" t="s">
         <v>119</v>
       </c>
@@ -8222,8 +8165,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" s="122"/>
-      <c r="B18" s="123"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="20" t="s">
         <v>120</v>
       </c>
@@ -8236,8 +8179,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="122"/>
-      <c r="B19" s="123"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="124"/>
       <c r="C19" s="20" t="s">
         <v>113</v>
       </c>
@@ -8250,11 +8193,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="122"/>
-      <c r="B20" s="112" t="s">
+      <c r="A20" s="123"/>
+      <c r="B20" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="112"/>
+      <c r="C20" s="113"/>
       <c r="D20" s="94">
         <f>SUM(D16:D19)</f>
         <v>0</v>
@@ -8273,10 +8216,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="122">
+      <c r="A21" s="123">
         <v>4</v>
       </c>
-      <c r="B21" s="123" t="s">
+      <c r="B21" s="124" t="s">
         <v>121</v>
       </c>
       <c r="C21" s="20" t="s">
@@ -8291,8 +8234,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="122"/>
-      <c r="B22" s="123"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="20" t="s">
         <v>123</v>
       </c>
@@ -8305,8 +8248,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="122"/>
-      <c r="B23" s="123"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="124"/>
       <c r="C23" s="20" t="s">
         <v>113</v>
       </c>
@@ -8319,11 +8262,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
-      <c r="B24" s="112" t="s">
+      <c r="A24" s="123"/>
+      <c r="B24" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="112"/>
+      <c r="C24" s="113"/>
       <c r="D24" s="94">
         <f>SUM(D21:D23)</f>
         <v>0</v>
@@ -8342,11 +8285,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="112" t="s">
+      <c r="A25" s="113" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="112"/>
-      <c r="C25" s="112"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="94">
         <f>D9+D15+D20+D24</f>
         <v>0</v>
@@ -8365,10 +8308,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="122">
+      <c r="A26" s="123">
         <v>5</v>
       </c>
-      <c r="B26" s="123" t="s">
+      <c r="B26" s="124" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="20" t="s">
@@ -8383,8 +8326,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="122"/>
-      <c r="B27" s="123"/>
+      <c r="A27" s="123"/>
+      <c r="B27" s="124"/>
       <c r="C27" s="20" t="s">
         <v>126</v>
       </c>
@@ -8397,11 +8340,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="122"/>
-      <c r="B28" s="112" t="s">
+      <c r="A28" s="123"/>
+      <c r="B28" s="113" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="112"/>
+      <c r="C28" s="113"/>
       <c r="D28" s="94">
         <f>SUM(D26:D27)</f>
         <v>0</v>
@@ -8420,11 +8363,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="112" t="s">
+      <c r="A29" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="B29" s="112"/>
-      <c r="C29" s="112"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="113"/>
       <c r="D29" s="94">
         <f>D25+D28</f>
         <v>0</v>
@@ -8508,24 +8451,24 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="115" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="116" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>62</v>
       </c>
@@ -8535,7 +8478,7 @@
       <c r="E4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="116"/>
+      <c r="F4" s="117"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -8663,10 +8606,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="112"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="94">
         <f>SUM(C6:C12)</f>
         <v>0</v>
@@ -8715,10 +8658,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="112" t="s">
+      <c r="A16" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="112"/>
+      <c r="B16" s="113"/>
       <c r="C16" s="94">
         <f>SUM(C14:C15)</f>
         <v>0</v>
@@ -9245,30 +9188,30 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117" t="s">
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="30" t="s">
         <v>62</v>
       </c>
@@ -9348,7 +9291,7 @@
       <c r="I7" s="37"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="124">
+      <c r="A8" s="125">
         <v>3</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -9363,7 +9306,7 @@
       <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="20" t="s">
         <v>234</v>
       </c>
@@ -9470,13 +9413,13 @@
     <mergeCell ref="D3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:I8 G10:I13">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="notBetween">
       <formula>0</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notBetween">
       <formula>0</formula>
       <formula>4</formula>
     </cfRule>
@@ -9548,28 +9491,28 @@
       <c r="A6" s="21"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="117" t="s">
+      <c r="A7" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="118" t="s">
         <v>330</v>
       </c>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="118" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117" t="s">
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="117"/>
+      <c r="A8" s="118"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="30" t="s">
         <v>153</v>
       </c>
@@ -9579,7 +9522,7 @@
       <c r="F8" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="117"/>
+      <c r="G8" s="118"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
@@ -9630,8 +9573,8 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="112"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="36">
         <f>COUNTIFS(B10:B11,"*",D10:D11,"V")</f>
         <v>0</v>
@@ -9671,10 +9614,10 @@
     <mergeCell ref="D7:F7"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:F11">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:F11" xr:uid="{00000000-0002-0000-1400-000000000000}">
@@ -9694,13 +9637,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9749,28 +9692,28 @@
       <c r="A6" s="21"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="117" t="s">
+      <c r="A7" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="118" t="s">
         <v>330</v>
       </c>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="118" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117" t="s">
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="117"/>
+      <c r="A8" s="118"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="30" t="s">
         <v>153</v>
       </c>
@@ -9780,7 +9723,7 @@
       <c r="F8" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="117"/>
+      <c r="G8" s="118"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
@@ -9818,8 +9761,8 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
-        <v>2</v>
+      <c r="A11" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -9827,147 +9770,57 @@
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="28"/>
-      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="34">
-        <v>3</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="I12" s="5"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="36">
+        <f>COUNTIFS(B10:B11,"*",D10:D11,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="36">
+        <f>COUNTIFS(B10:B11,"*",E10:E11,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="36">
+        <f>COUNTIFS(B10:B11,"*",F10:F11,"V")</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="55"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="34">
-        <v>4</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="21"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
-        <v>5</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
-        <v>6</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="34">
-        <v>7</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="109"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="36">
-        <f>COUNTIFS(B10:B17,"*",D10:D17,"V")</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="36">
-        <f>COUNTIFS(B10:B17,"*",E10:E17,"V")</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="36">
-        <f>COUNTIFS(B10:B17,"*",F10:F17,"V")</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="55"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="57"/>
-    </row>
-    <row r="21" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="s">
+      <c r="D14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="78" t="s">
         <v>307</v>
       </c>
-      <c r="D21" s="56"/>
+      <c r="D15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:F7"/>
   </mergeCells>
-  <conditionalFormatting sqref="D17:F17">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+  <conditionalFormatting sqref="D11:F11">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F10">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:F11">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:F12">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13:F13">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:F14">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15:F15">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:F16">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:F17" xr:uid="{00000000-0002-0000-1500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:F11" xr:uid="{00000000-0002-0000-1500-000000000000}">
       <formula1>$B$4:$B$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -10014,26 +9867,26 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>62</v>
       </c>
@@ -10108,7 +9961,7 @@
       <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="124">
+      <c r="A8" s="125">
         <v>3</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -10122,7 +9975,7 @@
       <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="20" t="s">
         <v>234</v>
       </c>
@@ -10261,24 +10114,24 @@
       <c r="A4" s="51"/>
     </row>
     <row r="5" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117" t="s">
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="117"/>
+      <c r="A6" s="118"/>
       <c r="B6" s="30" t="s">
         <v>160</v>
       </c>
@@ -10300,7 +10153,7 @@
       <c r="H6" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="I6" s="117"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
@@ -10431,21 +10284,21 @@
       <c r="A17" s="51"/>
     </row>
     <row r="18" spans="1:6" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="119" t="s">
+      <c r="A18" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="B18" s="119" t="s">
+      <c r="B18" s="120" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="120" t="s">
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="121" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="119"/>
+      <c r="A19" s="120"/>
       <c r="B19" s="26" t="s">
         <v>163</v>
       </c>
@@ -10458,7 +10311,7 @@
       <c r="E19" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="F19" s="121"/>
+      <c r="F19" s="122"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="32">
@@ -10529,20 +10382,20 @@
       <c r="A27" s="51"/>
     </row>
     <row r="28" spans="1:6" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="117" t="s">
+      <c r="C28" s="118"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="117"/>
+      <c r="A29" s="118"/>
       <c r="B29" s="30" t="s">
         <v>173</v>
       </c>
@@ -10552,7 +10405,7 @@
       <c r="D29" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="117"/>
+      <c r="E29" s="118"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="32">
@@ -10601,20 +10454,20 @@
       <c r="A35" s="51"/>
     </row>
     <row r="36" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="117" t="s">
+      <c r="A36" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="113" t="s">
+      <c r="B36" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="126"/>
-      <c r="D36" s="114"/>
-      <c r="E36" s="117" t="s">
+      <c r="C36" s="127"/>
+      <c r="D36" s="115"/>
+      <c r="E36" s="118" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="117"/>
+      <c r="A37" s="118"/>
       <c r="B37" s="30" t="s">
         <v>172</v>
       </c>
@@ -10624,7 +10477,7 @@
       <c r="D37" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="E37" s="117"/>
+      <c r="E37" s="118"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="32">
@@ -10682,24 +10535,24 @@
       <c r="A44" s="51"/>
     </row>
     <row r="45" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="117" t="s">
+      <c r="A45" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B45" s="117" t="s">
+      <c r="B45" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="C45" s="117"/>
-      <c r="D45" s="117"/>
-      <c r="E45" s="117"/>
-      <c r="F45" s="117"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="117"/>
-      <c r="I45" s="117" t="s">
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="118"/>
+      <c r="I45" s="118" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="117"/>
+      <c r="A46" s="118"/>
       <c r="B46" s="30" t="s">
         <v>177</v>
       </c>
@@ -10721,7 +10574,7 @@
       <c r="H46" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="I46" s="117"/>
+      <c r="I46" s="118"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="32">
@@ -10855,22 +10708,22 @@
       <c r="A57" s="51"/>
     </row>
     <row r="58" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="117" t="s">
+      <c r="A58" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B58" s="117" t="s">
+      <c r="B58" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="C58" s="117"/>
-      <c r="D58" s="117"/>
-      <c r="E58" s="117"/>
-      <c r="F58" s="117"/>
-      <c r="G58" s="115" t="s">
+      <c r="C58" s="118"/>
+      <c r="D58" s="118"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="118"/>
+      <c r="G58" s="116" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="117"/>
+      <c r="A59" s="118"/>
       <c r="B59" s="30" t="s">
         <v>179</v>
       </c>
@@ -10886,7 +10739,7 @@
       <c r="F59" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="G59" s="116"/>
+      <c r="G59" s="117"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="32">
@@ -10975,20 +10828,20 @@
       <c r="A68" s="51"/>
     </row>
     <row r="69" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="117" t="s">
+      <c r="A69" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="117" t="s">
+      <c r="B69" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="117"/>
-      <c r="D69" s="117"/>
-      <c r="E69" s="117" t="s">
+      <c r="C69" s="118"/>
+      <c r="D69" s="118"/>
+      <c r="E69" s="118" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="117"/>
+      <c r="A70" s="118"/>
       <c r="B70" s="30" t="s">
         <v>172</v>
       </c>
@@ -10998,7 +10851,7 @@
       <c r="D70" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="E70" s="117"/>
+      <c r="E70" s="118"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="32">
@@ -11056,20 +10909,20 @@
       <c r="A77" s="51"/>
     </row>
     <row r="78" spans="1:7" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="117" t="s">
+      <c r="A78" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B78" s="117" t="s">
+      <c r="B78" s="118" t="s">
         <v>182</v>
       </c>
-      <c r="C78" s="117"/>
-      <c r="D78" s="117"/>
-      <c r="E78" s="117" t="s">
+      <c r="C78" s="118"/>
+      <c r="D78" s="118"/>
+      <c r="E78" s="118" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="117"/>
+      <c r="A79" s="118"/>
       <c r="B79" s="30" t="s">
         <v>173</v>
       </c>
@@ -11079,7 +10932,7 @@
       <c r="D79" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="E79" s="117"/>
+      <c r="E79" s="118"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="32">
@@ -11184,26 +11037,26 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>60</v>
       </c>
@@ -11417,21 +11270,21 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:6" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>353</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>60</v>
       </c>
@@ -11614,21 +11467,21 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:6" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>60</v>
       </c>
@@ -11796,26 +11649,26 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>60</v>
       </c>
@@ -12054,22 +11907,22 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="118" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="30" t="s">
         <v>195</v>
       </c>
@@ -12211,7 +12064,7 @@
       <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12370,7 +12223,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
+      <c r="A15" s="100">
         <v>1</v>
       </c>
       <c r="B15" s="28"/>
@@ -12382,7 +12235,7 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="34">
+      <c r="A16" s="100">
         <v>2</v>
       </c>
       <c r="B16" s="28"/>
@@ -12391,14 +12244,13 @@
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="I16" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D15:D16" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D15:D16" xr:uid="{915715FB-2090-4C2D-B9BE-4CB33D923064}">
       <formula1>$B$4:$B$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:E16" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:E16" xr:uid="{C582888E-200D-4858-BEA3-499CCA13AC10}">
       <formula1>$C$4:$C$6</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0200-000002000000}">
@@ -12445,25 +12297,25 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="117" t="s">
+      <c r="A3" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="118" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="118" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
     </row>
     <row r="4" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="30" t="s">
         <v>208</v>
       </c>
@@ -12662,24 +12514,24 @@
       <c r="A2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="119" t="s">
+      <c r="A3" s="120" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="120" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="120" t="s">
         <v>211</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119" t="s">
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
-      <c r="B4" s="119"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="120"/>
       <c r="C4" s="26" t="s">
         <v>62</v>
       </c>
@@ -12689,7 +12541,7 @@
       <c r="E4" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="119"/>
+      <c r="F4" s="120"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
@@ -12847,10 +12699,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="112" t="s">
+      <c r="A15" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="127"/>
+      <c r="B15" s="128"/>
       <c r="C15" s="36">
         <f>SUM(C6:C14)</f>
         <v>0</v>
@@ -12961,10 +12813,10 @@
       <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="128" t="s">
+      <c r="A7" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="129"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="22">
         <f>COUNTA(C5:C6)</f>
         <v>0</v>
@@ -13054,11 +12906,11 @@
       <c r="A6" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="131" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="133"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47">
@@ -13101,10 +12953,10 @@
       <c r="D11" s="45"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="133" t="s">
+      <c r="A12" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="133"/>
+      <c r="B12" s="134"/>
       <c r="C12" s="47">
         <f>COUNTA(B7:B11)</f>
         <v>0</v>
@@ -13196,11 +13048,11 @@
       <c r="A6" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="131" t="s">
         <v>252</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="133"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47">
@@ -13219,10 +13071,10 @@
       <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="47">
         <f>COUNTA(B7:B8)</f>
         <v>0</v>
@@ -13314,11 +13166,11 @@
       <c r="A6" s="49" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="131" t="s">
         <v>243</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="133"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47">
@@ -13337,10 +13189,10 @@
       <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="47">
         <f>COUNTA(B7:B8)</f>
         <v>0</v>
@@ -13432,11 +13284,11 @@
       <c r="A6" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="131" t="s">
         <v>244</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="133"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47">
@@ -13455,10 +13307,10 @@
       <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="133"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="47">
         <f>COUNTA(B7:B8)</f>
         <v>0</v>
@@ -13594,7 +13446,7 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="100">
         <v>1</v>
       </c>
       <c r="B8" s="28"/>
@@ -13606,16 +13458,14 @@
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
-        <v>2</v>
+      <c r="A9" s="100" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13637,7 +13487,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13710,7 +13560,7 @@
       <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="100">
         <v>1</v>
       </c>
       <c r="B6" s="28"/>
@@ -13724,18 +13574,13 @@
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="34">
-        <v>2</v>
+      <c r="A7" s="100" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13776,56 +13621,56 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="107" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="107" t="s">
+      <c r="A3" s="108" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107" t="s">
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="107"/>
-      <c r="B4" s="107"/>
-      <c r="C4" s="107" t="s">
+      <c r="A4" s="108"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107" t="s">
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107" t="s">
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="107"/>
-      <c r="O4" s="107"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="107"/>
-      <c r="B5" s="107"/>
+      <c r="A5" s="108"/>
+      <c r="B5" s="108"/>
       <c r="C5" s="25" t="s">
         <v>32</v>
       </c>
@@ -13862,7 +13707,7 @@
       <c r="N5" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="107"/>
+      <c r="O5" s="108"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="32">
@@ -14104,10 +13949,10 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="106"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="22">
         <f>SUM(C7:C14)</f>
         <v>0</v>
@@ -14188,7 +14033,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14250,30 +14095,30 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="108" t="s">
+      <c r="A11" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="109" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108" t="s">
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="108" t="s">
+      <c r="G11" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="108" t="s">
+      <c r="H11" s="109" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="108"/>
-      <c r="B12" s="108"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="29" t="s">
         <v>55</v>
       </c>
@@ -14283,9 +14128,9 @@
       <c r="E12" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="F12" s="108"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
@@ -14357,10 +14202,10 @@
     <mergeCell ref="F11:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="C14:E14">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:E15">
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:E15" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -14382,8 +14227,8 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A62" sqref="A62:B63"/>
     </sheetView>
   </sheetViews>
@@ -14405,28 +14250,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="113" t="s">
+      <c r="D3" s="115"/>
+      <c r="E3" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="113" t="s">
+      <c r="F3" s="115"/>
+      <c r="G3" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="114"/>
+      <c r="H3" s="115"/>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="30" t="s">
         <v>70</v>
       </c>
@@ -14473,16 +14318,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="110" t="s">
         <v>223</v>
       </c>
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="112"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
@@ -14545,10 +14390,10 @@
       <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="111"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="36">
         <f t="shared" ref="C12:F12" si="0">SUM(C7:C11)</f>
         <v>0</v>
@@ -14565,23 +14410,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="109">
+      <c r="G12" s="110">
         <f>SUM(G11:H11)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="111"/>
+      <c r="H12" s="112"/>
     </row>
     <row r="13" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="111"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="112"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -14644,10 +14489,10 @@
       <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="111"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="36">
         <f t="shared" ref="C19:F19" si="1">SUM(C14:C18)</f>
         <v>0</v>
@@ -14664,23 +14509,23 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="109">
+      <c r="G19" s="110">
         <f>SUM(G18:H18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="111"/>
+      <c r="H19" s="112"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="110" t="s">
         <v>229</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="111"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="112"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
@@ -14743,10 +14588,10 @@
       <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="111"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="36">
         <f t="shared" ref="C26:F26" si="2">SUM(C21:C25)</f>
         <v>0</v>
@@ -14763,23 +14608,23 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G26" s="109">
+      <c r="G26" s="110">
         <f>SUM(G25:H25)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="111"/>
+      <c r="H26" s="112"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="109" t="s">
+      <c r="A27" s="110" t="s">
         <v>332</v>
       </c>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="111"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="112"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
@@ -14842,10 +14687,10 @@
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="109" t="s">
+      <c r="A33" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="111"/>
+      <c r="B33" s="112"/>
       <c r="C33" s="36">
         <f t="shared" ref="C33:F33" si="3">SUM(C28:C32)</f>
         <v>0</v>
@@ -14862,23 +14707,23 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G33" s="109">
+      <c r="G33" s="110">
         <f>SUM(G32:H32)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="111"/>
+      <c r="H33" s="112"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="110" t="s">
         <v>337</v>
       </c>
-      <c r="B34" s="110"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="111"/>
+      <c r="B34" s="111"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="111"/>
+      <c r="E34" s="111"/>
+      <c r="F34" s="111"/>
+      <c r="G34" s="111"/>
+      <c r="H34" s="112"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
@@ -14941,10 +14786,10 @@
       <c r="H39" s="27"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="109" t="s">
+      <c r="A40" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="111"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="36">
         <f t="shared" ref="C40:F40" si="4">SUM(C35:C39)</f>
         <v>0</v>
@@ -14961,23 +14806,23 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G40" s="109">
+      <c r="G40" s="110">
         <f>SUM(G39:H39)</f>
         <v>0</v>
       </c>
-      <c r="H40" s="111"/>
+      <c r="H40" s="112"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="109" t="s">
+      <c r="A41" s="110" t="s">
         <v>225</v>
       </c>
-      <c r="B41" s="110"/>
-      <c r="C41" s="110"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="110"/>
-      <c r="F41" s="110"/>
-      <c r="G41" s="110"/>
-      <c r="H41" s="111"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="112"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
@@ -15040,10 +14885,10 @@
       <c r="H46" s="27"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="109" t="s">
+      <c r="A47" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="111"/>
+      <c r="B47" s="112"/>
       <c r="C47" s="36">
         <f t="shared" ref="C47:F47" si="5">SUM(C42:C46)</f>
         <v>0</v>
@@ -15060,23 +14905,23 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G47" s="109">
+      <c r="G47" s="110">
         <f>SUM(G46:H46)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="111"/>
+      <c r="H47" s="112"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="109" t="s">
+      <c r="A48" s="110" t="s">
         <v>226</v>
       </c>
-      <c r="B48" s="110"/>
-      <c r="C48" s="110"/>
-      <c r="D48" s="110"/>
-      <c r="E48" s="110"/>
-      <c r="F48" s="110"/>
-      <c r="G48" s="110"/>
-      <c r="H48" s="111"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="111"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="111"/>
+      <c r="G48" s="111"/>
+      <c r="H48" s="112"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="s">
@@ -15139,10 +14984,10 @@
       <c r="H53" s="27"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="109" t="s">
+      <c r="A54" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B54" s="111"/>
+      <c r="B54" s="112"/>
       <c r="C54" s="36">
         <f t="shared" ref="C54:F54" si="6">SUM(C49:C53)</f>
         <v>0</v>
@@ -15159,23 +15004,23 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G54" s="109">
+      <c r="G54" s="110">
         <f>SUM(G53:H53)</f>
         <v>0</v>
       </c>
-      <c r="H54" s="111"/>
+      <c r="H54" s="112"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="109" t="s">
+      <c r="A55" s="110" t="s">
         <v>227</v>
       </c>
-      <c r="B55" s="110"/>
-      <c r="C55" s="110"/>
-      <c r="D55" s="110"/>
-      <c r="E55" s="110"/>
-      <c r="F55" s="110"/>
-      <c r="G55" s="110"/>
-      <c r="H55" s="111"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="111"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="111"/>
+      <c r="F55" s="111"/>
+      <c r="G55" s="111"/>
+      <c r="H55" s="112"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="s">
@@ -15238,10 +15083,10 @@
       <c r="H60" s="27"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="109" t="s">
+      <c r="A61" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B61" s="111"/>
+      <c r="B61" s="112"/>
       <c r="C61" s="36">
         <f t="shared" ref="C61:F61" si="7">SUM(C56:C60)</f>
         <v>0</v>
@@ -15258,30 +15103,30 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G61" s="109">
+      <c r="G61" s="110">
         <f>SUM(G60:H60)</f>
         <v>0</v>
       </c>
-      <c r="H61" s="111"/>
+      <c r="H61" s="112"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="112" t="s">
+      <c r="A62" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="112"/>
-      <c r="C62" s="112">
+      <c r="B62" s="113"/>
+      <c r="C62" s="113">
         <f>C12+C19+C61+C40+C47+C54+C26+C33</f>
         <v>0</v>
       </c>
-      <c r="D62" s="112">
+      <c r="D62" s="113">
         <f>D12+D19+D61+D40+D47+D54+D26+D33</f>
         <v>0</v>
       </c>
-      <c r="E62" s="112">
+      <c r="E62" s="113">
         <f>E12+E19+E61+E40+E47+E54+E26+E33</f>
         <v>0</v>
       </c>
-      <c r="F62" s="112">
+      <c r="F62" s="113">
         <f>F12+F19+F61+F40+F47+F54+F26+F33</f>
         <v>0</v>
       </c>
@@ -15295,17 +15140,17 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="112"/>
-      <c r="B63" s="112"/>
-      <c r="C63" s="112"/>
-      <c r="D63" s="112"/>
-      <c r="E63" s="112"/>
-      <c r="F63" s="112"/>
-      <c r="G63" s="109">
+      <c r="A63" s="113"/>
+      <c r="B63" s="113"/>
+      <c r="C63" s="113"/>
+      <c r="D63" s="113"/>
+      <c r="E63" s="113"/>
+      <c r="F63" s="113"/>
+      <c r="G63" s="110">
         <f>G62+H62</f>
         <v>0</v>
       </c>
-      <c r="H63" s="111"/>
+      <c r="H63" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -15364,7 +15209,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15437,10 +15282,10 @@
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="112"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="36">
         <f>SUM(C5:C6)</f>
         <v>0</v>

</xml_diff>

<commit_message>
kuantitatif export Akademik selesai
</commit_message>
<xml_diff>
--- a/common/required/kriteria9/apt/template/kuantitatif_akademik.xlsx
+++ b/common/required/kriteria9/apt/template/kuantitatif_akademik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adryanev\Code\php\kriteria\common\required\kriteria9\apt\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D3FD9E-BDEB-4D2B-9F43-7551B99B5869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F31A2F-9A5F-4573-8C24-656B12F42035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="6930" windowWidth="15375" windowHeight="8085" tabRatio="839" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="839" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="14" r:id="rId1"/>
@@ -2064,7 +2064,7 @@
     <author>Suharyadi</author>
   </authors>
   <commentList>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2000-000001000000}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -4655,6 +4655,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4663,15 +4672,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4691,9 +4691,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4704,6 +4701,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5231,62 +5231,62 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="101"/>
-      <c r="W2" s="101"/>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="101"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="102"/>
-      <c r="T3" s="102"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="102"/>
-      <c r="W3" s="102"/>
-      <c r="X3" s="102"/>
-      <c r="Y3" s="102"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="105"/>
+      <c r="Y3" s="105"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -5316,33 +5316,33 @@
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="106" t="s">
+      <c r="A5" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="103"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -5383,23 +5383,23 @@
       <c r="G7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103"/>
-      <c r="O7" s="103"/>
-      <c r="P7" s="103"/>
-      <c r="Q7" s="103"/>
-      <c r="R7" s="103"/>
-      <c r="S7" s="103"/>
-      <c r="T7" s="103"/>
-      <c r="U7" s="103"/>
-      <c r="V7" s="103"/>
-      <c r="W7" s="103"/>
-      <c r="X7" s="103"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="106"/>
+      <c r="Q7" s="106"/>
+      <c r="R7" s="106"/>
+      <c r="S7" s="106"/>
+      <c r="T7" s="106"/>
+      <c r="U7" s="106"/>
+      <c r="V7" s="106"/>
+      <c r="W7" s="106"/>
+      <c r="X7" s="106"/>
       <c r="Y7" s="11"/>
     </row>
     <row r="8" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5441,13 +5441,13 @@
       <c r="G9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -5640,15 +5640,15 @@
       <c r="G16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="104"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
+      <c r="P16" s="102"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
@@ -5868,23 +5868,23 @@
       <c r="G24" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
-      <c r="K24" s="104"/>
-      <c r="L24" s="104"/>
-      <c r="M24" s="104"/>
-      <c r="N24" s="104"/>
-      <c r="O24" s="104"/>
-      <c r="P24" s="104"/>
-      <c r="Q24" s="104"/>
-      <c r="R24" s="104"/>
-      <c r="S24" s="104"/>
-      <c r="T24" s="104"/>
-      <c r="U24" s="104"/>
-      <c r="V24" s="104"/>
-      <c r="W24" s="104"/>
-      <c r="X24" s="104"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="102"/>
+      <c r="Q24" s="102"/>
+      <c r="R24" s="102"/>
+      <c r="S24" s="102"/>
+      <c r="T24" s="102"/>
+      <c r="U24" s="102"/>
+      <c r="V24" s="102"/>
+      <c r="W24" s="102"/>
+      <c r="X24" s="102"/>
       <c r="Y24" s="11"/>
     </row>
     <row r="25" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5922,23 +5922,23 @@
       <c r="E26" s="11"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
-      <c r="K26" s="104"/>
-      <c r="L26" s="104"/>
-      <c r="M26" s="104"/>
-      <c r="N26" s="104"/>
-      <c r="O26" s="104"/>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
-      <c r="S26" s="104"/>
-      <c r="T26" s="104"/>
-      <c r="U26" s="104"/>
-      <c r="V26" s="104"/>
-      <c r="W26" s="104"/>
-      <c r="X26" s="104"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="102"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="102"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="102"/>
+      <c r="Q26" s="102"/>
+      <c r="R26" s="102"/>
+      <c r="S26" s="102"/>
+      <c r="T26" s="102"/>
+      <c r="U26" s="102"/>
+      <c r="V26" s="102"/>
+      <c r="W26" s="102"/>
+      <c r="X26" s="102"/>
       <c r="Y26" s="11"/>
     </row>
     <row r="27" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5980,13 +5980,13 @@
       <c r="G28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="104"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="104"/>
-      <c r="K28" s="104"/>
-      <c r="L28" s="104"/>
-      <c r="M28" s="104"/>
-      <c r="N28" s="104"/>
+      <c r="H28" s="102"/>
+      <c r="I28" s="102"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102"/>
+      <c r="N28" s="102"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="13"/>
@@ -6038,16 +6038,16 @@
       <c r="G30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
-      <c r="K30" s="104"/>
-      <c r="L30" s="104"/>
-      <c r="M30" s="104"/>
-      <c r="N30" s="104"/>
-      <c r="O30" s="104"/>
-      <c r="P30" s="104"/>
-      <c r="Q30" s="104"/>
+      <c r="H30" s="102"/>
+      <c r="I30" s="102"/>
+      <c r="J30" s="102"/>
+      <c r="K30" s="102"/>
+      <c r="L30" s="102"/>
+      <c r="M30" s="102"/>
+      <c r="N30" s="102"/>
+      <c r="O30" s="102"/>
+      <c r="P30" s="102"/>
+      <c r="Q30" s="102"/>
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
@@ -6096,15 +6096,15 @@
       <c r="G32" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="104"/>
-      <c r="L32" s="104"/>
-      <c r="M32" s="104"/>
-      <c r="N32" s="104"/>
-      <c r="O32" s="104"/>
-      <c r="P32" s="104"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
+      <c r="J32" s="102"/>
+      <c r="K32" s="102"/>
+      <c r="L32" s="102"/>
+      <c r="M32" s="102"/>
+      <c r="N32" s="102"/>
+      <c r="O32" s="102"/>
+      <c r="P32" s="102"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
       <c r="S32" s="13"/>
@@ -6154,15 +6154,15 @@
       <c r="G34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="104"/>
-      <c r="I34" s="104"/>
-      <c r="J34" s="104"/>
-      <c r="K34" s="104"/>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-      <c r="N34" s="104"/>
-      <c r="O34" s="104"/>
-      <c r="P34" s="104"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="102"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="102"/>
+      <c r="O34" s="102"/>
+      <c r="P34" s="102"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
@@ -6212,11 +6212,11 @@
       <c r="G36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H36" s="104"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="104"/>
-      <c r="K36" s="104"/>
-      <c r="L36" s="104"/>
+      <c r="H36" s="102"/>
+      <c r="I36" s="102"/>
+      <c r="J36" s="102"/>
+      <c r="K36" s="102"/>
+      <c r="L36" s="102"/>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
@@ -6328,15 +6328,15 @@
       <c r="G40" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="104"/>
-      <c r="I40" s="104"/>
-      <c r="J40" s="104"/>
-      <c r="K40" s="104"/>
-      <c r="L40" s="104"/>
-      <c r="M40" s="104"/>
-      <c r="N40" s="104"/>
-      <c r="O40" s="104"/>
-      <c r="P40" s="104"/>
+      <c r="H40" s="102"/>
+      <c r="I40" s="102"/>
+      <c r="J40" s="102"/>
+      <c r="K40" s="102"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="102"/>
+      <c r="N40" s="102"/>
+      <c r="O40" s="102"/>
+      <c r="P40" s="102"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
@@ -6515,12 +6515,12 @@
       <c r="R46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S46" s="104"/>
-      <c r="T46" s="104"/>
-      <c r="U46" s="104"/>
-      <c r="V46" s="104"/>
-      <c r="W46" s="104"/>
-      <c r="X46" s="104"/>
+      <c r="S46" s="102"/>
+      <c r="T46" s="102"/>
+      <c r="U46" s="102"/>
+      <c r="V46" s="102"/>
+      <c r="W46" s="102"/>
+      <c r="X46" s="102"/>
       <c r="Y46" s="11"/>
     </row>
     <row r="47" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6575,12 +6575,12 @@
       <c r="R48" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S48" s="105">
+      <c r="S48" s="101">
         <f ca="1">TODAY()</f>
-        <v>44200</v>
-      </c>
-      <c r="T48" s="105"/>
-      <c r="U48" s="105"/>
+        <v>44202</v>
+      </c>
+      <c r="T48" s="101"/>
+      <c r="U48" s="101"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
@@ -6652,6 +6652,11 @@
     <protectedRange sqref="H7:I7" name="Nama PT"/>
   </protectedRanges>
   <mergeCells count="16">
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="H7:X7"/>
+    <mergeCell ref="H9:N9"/>
+    <mergeCell ref="H16:P16"/>
     <mergeCell ref="S48:U48"/>
     <mergeCell ref="H40:P40"/>
     <mergeCell ref="S46:X46"/>
@@ -6663,11 +6668,6 @@
     <mergeCell ref="H32:P32"/>
     <mergeCell ref="H34:P34"/>
     <mergeCell ref="H36:L36"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="H7:X7"/>
-    <mergeCell ref="H9:N9"/>
-    <mergeCell ref="H16:P16"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16:P16" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -6721,7 +6721,7 @@
       <c r="A3" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="115" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="118" t="s">
@@ -6735,7 +6735,7 @@
     </row>
     <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="118"/>
-      <c r="B4" s="117"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="30" t="s">
         <v>74</v>
       </c>
@@ -6794,10 +6794,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="113" t="s">
+      <c r="A8" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="113"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="36">
         <f>SUM(C6:C7)</f>
         <v>0</v>
@@ -6978,10 +6978,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7100,10 +7100,10 @@
       <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="113"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="34">
         <f>SUM(C5:C6)</f>
         <v>0</v>
@@ -7275,10 +7275,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7405,10 +7405,10 @@
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="113"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="36">
         <f>SUM(C5:C6)</f>
         <v>0</v>
@@ -7561,10 +7561,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7725,10 +7725,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="113"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7769,7 +7769,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -7881,10 +7881,10 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29:C29"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8014,10 +8014,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="123"/>
-      <c r="B9" s="113" t="s">
+      <c r="B9" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="113"/>
+      <c r="C9" s="117"/>
       <c r="D9" s="94">
         <f>SUM(D6:D8)</f>
         <v>0</v>
@@ -8111,10 +8111,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="123"/>
-      <c r="B15" s="113" t="s">
+      <c r="B15" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="113"/>
+      <c r="C15" s="117"/>
       <c r="D15" s="94">
         <f>SUM(D10:D14)</f>
         <v>0</v>
@@ -8194,10 +8194,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="123"/>
-      <c r="B20" s="113" t="s">
+      <c r="B20" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="113"/>
+      <c r="C20" s="117"/>
       <c r="D20" s="94">
         <f>SUM(D16:D19)</f>
         <v>0</v>
@@ -8263,10 +8263,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="123"/>
-      <c r="B24" s="113" t="s">
+      <c r="B24" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="113"/>
+      <c r="C24" s="117"/>
       <c r="D24" s="94">
         <f>SUM(D21:D23)</f>
         <v>0</v>
@@ -8285,11 +8285,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="113" t="s">
+      <c r="A25" s="117" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="117"/>
       <c r="D25" s="94">
         <f>D9+D15+D20+D24</f>
         <v>0</v>
@@ -8341,10 +8341,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="123"/>
-      <c r="B28" s="113" t="s">
+      <c r="B28" s="117" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="113"/>
+      <c r="C28" s="117"/>
       <c r="D28" s="94">
         <f>SUM(D26:D27)</f>
         <v>0</v>
@@ -8363,11 +8363,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="113" t="s">
+      <c r="A29" s="117" t="s">
         <v>232</v>
       </c>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
       <c r="D29" s="94">
         <f>D25+D28</f>
         <v>0</v>
@@ -8387,6 +8387,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="B20:C20"/>
@@ -8398,17 +8409,6 @@
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="D3" s="118"/>
       <c r="E3" s="118"/>
-      <c r="F3" s="116" t="s">
+      <c r="F3" s="115" t="s">
         <v>354</v>
       </c>
     </row>
@@ -8478,7 +8478,7 @@
       <c r="E4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="117"/>
+      <c r="F4" s="116"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -8606,10 +8606,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="113"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="94">
         <f>SUM(C6:C12)</f>
         <v>0</v>
@@ -8658,10 +8658,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="113"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="94">
         <f>SUM(C14:C15)</f>
         <v>0</v>
@@ -9161,10 +9161,10 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9573,8 +9573,8 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="117"/>
       <c r="D12" s="36">
         <f>COUNTIFS(B10:B11,"*",D10:D11,"V")</f>
         <v>0</v>
@@ -9643,7 +9643,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:G16"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9843,7 +9843,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10457,11 +10457,11 @@
       <c r="A36" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="114" t="s">
+      <c r="B36" s="113" t="s">
         <v>169</v>
       </c>
       <c r="C36" s="127"/>
-      <c r="D36" s="115"/>
+      <c r="D36" s="114"/>
       <c r="E36" s="118" t="s">
         <v>171</v>
       </c>
@@ -10718,7 +10718,7 @@
       <c r="D58" s="118"/>
       <c r="E58" s="118"/>
       <c r="F58" s="118"/>
-      <c r="G58" s="116" t="s">
+      <c r="G58" s="115" t="s">
         <v>183</v>
       </c>
     </row>
@@ -10739,7 +10739,7 @@
       <c r="F59" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="G59" s="117"/>
+      <c r="G59" s="116"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="32">
@@ -10971,6 +10971,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:E70"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="A78:A79"/>
     <mergeCell ref="B78:D78"/>
@@ -10980,21 +10995,6 @@
     <mergeCell ref="B45:H45"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="E36:E37"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
@@ -12699,7 +12699,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="117" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="128"/>
@@ -12839,13 +12839,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12921,52 +12921,28 @@
       <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="47">
-        <v>2</v>
+      <c r="A8" s="47" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="70"/>
       <c r="C8" s="48"/>
       <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
-        <v>3</v>
-      </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="45"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
-        <v>4</v>
-      </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="45"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="45"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="134" t="s">
+      <c r="A9" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="134"/>
-      <c r="C12" s="47">
-        <f>COUNTA(B7:B11)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="69"/>
+      <c r="B9" s="134"/>
+      <c r="C9" s="47">
+        <f>COUNTA(B7:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
@@ -13338,7 +13314,7 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -14250,28 +14226,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="115"/>
-      <c r="E3" s="114" t="s">
+      <c r="D3" s="114"/>
+      <c r="E3" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="115"/>
-      <c r="G3" s="114" t="s">
+      <c r="F3" s="114"/>
+      <c r="G3" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="115"/>
+      <c r="H3" s="114"/>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="117"/>
+      <c r="A4" s="116"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="30" t="s">
         <v>70</v>
       </c>
@@ -15110,23 +15086,23 @@
       <c r="H61" s="112"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="113" t="s">
+      <c r="A62" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="113"/>
-      <c r="C62" s="113">
+      <c r="B62" s="117"/>
+      <c r="C62" s="117">
         <f>C12+C19+C61+C40+C47+C54+C26+C33</f>
         <v>0</v>
       </c>
-      <c r="D62" s="113">
+      <c r="D62" s="117">
         <f>D12+D19+D61+D40+D47+D54+D26+D33</f>
         <v>0</v>
       </c>
-      <c r="E62" s="113">
+      <c r="E62" s="117">
         <f>E12+E19+E61+E40+E47+E54+E26+E33</f>
         <v>0</v>
       </c>
-      <c r="F62" s="113">
+      <c r="F62" s="117">
         <f>F12+F19+F61+F40+F47+F54+F26+F33</f>
         <v>0</v>
       </c>
@@ -15140,12 +15116,12 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="113"/>
-      <c r="B63" s="113"/>
-      <c r="C63" s="113"/>
-      <c r="D63" s="113"/>
-      <c r="E63" s="113"/>
-      <c r="F63" s="113"/>
+      <c r="A63" s="117"/>
+      <c r="B63" s="117"/>
+      <c r="C63" s="117"/>
+      <c r="D63" s="117"/>
+      <c r="E63" s="117"/>
+      <c r="F63" s="117"/>
       <c r="G63" s="110">
         <f>G62+H62</f>
         <v>0</v>
@@ -15154,6 +15130,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="G3:H3"/>
@@ -15170,25 +15165,6 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A20:H20"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G40:H40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
@@ -15282,10 +15258,10 @@
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="113"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="36">
         <f>SUM(C5:C6)</f>
         <v>0</v>

</xml_diff>

<commit_message>
perbaiki expor kuantitatif institusi
</commit_message>
<xml_diff>
--- a/common/required/kriteria9/apt/template/kuantitatif_akademik.xlsx
+++ b/common/required/kriteria9/apt/template/kuantitatif_akademik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adryanev\Code\php\kriteria\common\required\kriteria9\apt\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F31A2F-9A5F-4573-8C24-656B12F42035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BE8E87-9457-4532-85A2-AB0C0CD17DFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="839" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="1395" windowWidth="21600" windowHeight="11505" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="14" r:id="rId1"/>
@@ -4655,15 +4655,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4672,6 +4663,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4691,6 +4691,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4701,9 +4704,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5187,7 +5187,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H7" sqref="H7:X7"/>
     </sheetView>
   </sheetViews>
@@ -5231,62 +5231,62 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="101"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="101"/>
+      <c r="X2" s="101"/>
+      <c r="Y2" s="101"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
-      <c r="Y3" s="105"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="102"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -5316,33 +5316,33 @@
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="106" t="s">
         <v>325</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="103"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="103"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="106"/>
+      <c r="T5" s="106"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="106"/>
+      <c r="X5" s="106"/>
+      <c r="Y5" s="106"/>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -5383,23 +5383,23 @@
       <c r="G7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="103"/>
+      <c r="V7" s="103"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="103"/>
       <c r="Y7" s="11"/>
     </row>
     <row r="8" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5441,13 +5441,13 @@
       <c r="G9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -5640,15 +5640,15 @@
       <c r="G16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="102"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="102"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="104"/>
+      <c r="M16" s="104"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="104"/>
+      <c r="P16" s="104"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
@@ -5868,23 +5868,23 @@
       <c r="G24" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="102"/>
-      <c r="N24" s="102"/>
-      <c r="O24" s="102"/>
-      <c r="P24" s="102"/>
-      <c r="Q24" s="102"/>
-      <c r="R24" s="102"/>
-      <c r="S24" s="102"/>
-      <c r="T24" s="102"/>
-      <c r="U24" s="102"/>
-      <c r="V24" s="102"/>
-      <c r="W24" s="102"/>
-      <c r="X24" s="102"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="104"/>
+      <c r="V24" s="104"/>
+      <c r="W24" s="104"/>
+      <c r="X24" s="104"/>
       <c r="Y24" s="11"/>
     </row>
     <row r="25" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5922,23 +5922,23 @@
       <c r="E26" s="11"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="102"/>
-      <c r="I26" s="102"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102"/>
-      <c r="L26" s="102"/>
-      <c r="M26" s="102"/>
-      <c r="N26" s="102"/>
-      <c r="O26" s="102"/>
-      <c r="P26" s="102"/>
-      <c r="Q26" s="102"/>
-      <c r="R26" s="102"/>
-      <c r="S26" s="102"/>
-      <c r="T26" s="102"/>
-      <c r="U26" s="102"/>
-      <c r="V26" s="102"/>
-      <c r="W26" s="102"/>
-      <c r="X26" s="102"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="104"/>
+      <c r="M26" s="104"/>
+      <c r="N26" s="104"/>
+      <c r="O26" s="104"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="104"/>
+      <c r="U26" s="104"/>
+      <c r="V26" s="104"/>
+      <c r="W26" s="104"/>
+      <c r="X26" s="104"/>
       <c r="Y26" s="11"/>
     </row>
     <row r="27" spans="1:25" s="9" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5980,13 +5980,13 @@
       <c r="G28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="102"/>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
-      <c r="K28" s="102"/>
-      <c r="L28" s="102"/>
-      <c r="M28" s="102"/>
-      <c r="N28" s="102"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="104"/>
+      <c r="N28" s="104"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="13"/>
@@ -6038,16 +6038,16 @@
       <c r="G30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="102"/>
-      <c r="I30" s="102"/>
-      <c r="J30" s="102"/>
-      <c r="K30" s="102"/>
-      <c r="L30" s="102"/>
-      <c r="M30" s="102"/>
-      <c r="N30" s="102"/>
-      <c r="O30" s="102"/>
-      <c r="P30" s="102"/>
-      <c r="Q30" s="102"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="104"/>
+      <c r="L30" s="104"/>
+      <c r="M30" s="104"/>
+      <c r="N30" s="104"/>
+      <c r="O30" s="104"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
@@ -6096,15 +6096,15 @@
       <c r="G32" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="102"/>
-      <c r="K32" s="102"/>
-      <c r="L32" s="102"/>
-      <c r="M32" s="102"/>
-      <c r="N32" s="102"/>
-      <c r="O32" s="102"/>
-      <c r="P32" s="102"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="104"/>
+      <c r="N32" s="104"/>
+      <c r="O32" s="104"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
       <c r="S32" s="13"/>
@@ -6154,15 +6154,15 @@
       <c r="G34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="102"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
-      <c r="K34" s="102"/>
-      <c r="L34" s="102"/>
-      <c r="M34" s="102"/>
-      <c r="N34" s="102"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="102"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="104"/>
+      <c r="K34" s="104"/>
+      <c r="L34" s="104"/>
+      <c r="M34" s="104"/>
+      <c r="N34" s="104"/>
+      <c r="O34" s="104"/>
+      <c r="P34" s="104"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13"/>
@@ -6212,11 +6212,11 @@
       <c r="G36" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H36" s="102"/>
-      <c r="I36" s="102"/>
-      <c r="J36" s="102"/>
-      <c r="K36" s="102"/>
-      <c r="L36" s="102"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="104"/>
+      <c r="J36" s="104"/>
+      <c r="K36" s="104"/>
+      <c r="L36" s="104"/>
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
@@ -6328,15 +6328,15 @@
       <c r="G40" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="102"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
-      <c r="L40" s="102"/>
-      <c r="M40" s="102"/>
-      <c r="N40" s="102"/>
-      <c r="O40" s="102"/>
-      <c r="P40" s="102"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
+      <c r="L40" s="104"/>
+      <c r="M40" s="104"/>
+      <c r="N40" s="104"/>
+      <c r="O40" s="104"/>
+      <c r="P40" s="104"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
@@ -6515,12 +6515,12 @@
       <c r="R46" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S46" s="102"/>
-      <c r="T46" s="102"/>
-      <c r="U46" s="102"/>
-      <c r="V46" s="102"/>
-      <c r="W46" s="102"/>
-      <c r="X46" s="102"/>
+      <c r="S46" s="104"/>
+      <c r="T46" s="104"/>
+      <c r="U46" s="104"/>
+      <c r="V46" s="104"/>
+      <c r="W46" s="104"/>
+      <c r="X46" s="104"/>
       <c r="Y46" s="11"/>
     </row>
     <row r="47" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6575,12 +6575,12 @@
       <c r="R48" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S48" s="101">
+      <c r="S48" s="105">
         <f ca="1">TODAY()</f>
-        <v>44202</v>
-      </c>
-      <c r="T48" s="101"/>
-      <c r="U48" s="101"/>
+        <v>44272</v>
+      </c>
+      <c r="T48" s="105"/>
+      <c r="U48" s="105"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
@@ -6652,11 +6652,6 @@
     <protectedRange sqref="H7:I7" name="Nama PT"/>
   </protectedRanges>
   <mergeCells count="16">
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A3:Y3"/>
-    <mergeCell ref="H7:X7"/>
-    <mergeCell ref="H9:N9"/>
-    <mergeCell ref="H16:P16"/>
     <mergeCell ref="S48:U48"/>
     <mergeCell ref="H40:P40"/>
     <mergeCell ref="S46:X46"/>
@@ -6668,6 +6663,11 @@
     <mergeCell ref="H32:P32"/>
     <mergeCell ref="H34:P34"/>
     <mergeCell ref="H36:L36"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A3:Y3"/>
+    <mergeCell ref="H7:X7"/>
+    <mergeCell ref="H9:N9"/>
+    <mergeCell ref="H16:P16"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16:P16" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -6721,7 +6721,7 @@
       <c r="A3" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="118" t="s">
@@ -6735,7 +6735,7 @@
     </row>
     <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="118"/>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="30" t="s">
         <v>74</v>
       </c>
@@ -6794,10 +6794,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="117"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="36">
         <f>SUM(C6:C7)</f>
         <v>0</v>
@@ -6978,10 +6978,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7100,10 +7100,10 @@
       <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="34">
         <f>SUM(C5:C6)</f>
         <v>0</v>
@@ -7275,10 +7275,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7405,10 +7405,10 @@
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="36">
         <f>SUM(C5:C6)</f>
         <v>0</v>
@@ -7561,10 +7561,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -7725,10 +7725,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="36">
         <f>SUM(C6:C8)</f>
         <v>0</v>
@@ -8014,10 +8014,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="123"/>
-      <c r="B9" s="117" t="s">
+      <c r="B9" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="117"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="94">
         <f>SUM(D6:D8)</f>
         <v>0</v>
@@ -8111,10 +8111,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="123"/>
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="117"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="94">
         <f>SUM(D10:D14)</f>
         <v>0</v>
@@ -8194,10 +8194,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="123"/>
-      <c r="B20" s="117" t="s">
+      <c r="B20" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="117"/>
+      <c r="C20" s="113"/>
       <c r="D20" s="94">
         <f>SUM(D16:D19)</f>
         <v>0</v>
@@ -8263,10 +8263,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="123"/>
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="117"/>
+      <c r="C24" s="113"/>
       <c r="D24" s="94">
         <f>SUM(D21:D23)</f>
         <v>0</v>
@@ -8285,11 +8285,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="113" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="94">
         <f>D9+D15+D20+D24</f>
         <v>0</v>
@@ -8341,10 +8341,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="123"/>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="113" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="117"/>
+      <c r="C28" s="113"/>
       <c r="D28" s="94">
         <f>SUM(D26:D27)</f>
         <v>0</v>
@@ -8363,11 +8363,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="117" t="s">
+      <c r="A29" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="113"/>
       <c r="D29" s="94">
         <f>D25+D28</f>
         <v>0</v>
@@ -8387,6 +8387,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="A10:A15"/>
@@ -8398,17 +8409,6 @@
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="D3" s="118"/>
       <c r="E3" s="118"/>
-      <c r="F3" s="115" t="s">
+      <c r="F3" s="116" t="s">
         <v>354</v>
       </c>
     </row>
@@ -8478,7 +8478,7 @@
       <c r="E4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="116"/>
+      <c r="F4" s="117"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
@@ -8606,10 +8606,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="117"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="94">
         <f>SUM(C6:C12)</f>
         <v>0</v>
@@ -8658,10 +8658,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="117" t="s">
+      <c r="A16" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="117"/>
+      <c r="B16" s="113"/>
       <c r="C16" s="94">
         <f>SUM(C14:C15)</f>
         <v>0</v>
@@ -9573,8 +9573,8 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
-      <c r="B12" s="117"/>
-      <c r="C12" s="117"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="36">
         <f>COUNTIFS(B10:B11,"*",D10:D11,"V")</f>
         <v>0</v>
@@ -10457,11 +10457,11 @@
       <c r="A36" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="113" t="s">
+      <c r="B36" s="114" t="s">
         <v>169</v>
       </c>
       <c r="C36" s="127"/>
-      <c r="D36" s="114"/>
+      <c r="D36" s="115"/>
       <c r="E36" s="118" t="s">
         <v>171</v>
       </c>
@@ -10718,7 +10718,7 @@
       <c r="D58" s="118"/>
       <c r="E58" s="118"/>
       <c r="F58" s="118"/>
-      <c r="G58" s="115" t="s">
+      <c r="G58" s="116" t="s">
         <v>183</v>
       </c>
     </row>
@@ -10739,7 +10739,7 @@
       <c r="F59" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="G59" s="116"/>
+      <c r="G59" s="117"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="32">
@@ -10971,6 +10971,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:E70"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:E18"/>
@@ -10980,21 +10995,6 @@
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="E36:E37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
@@ -12699,7 +12699,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="113" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="128"/>
@@ -13314,7 +13314,7 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -14226,28 +14226,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="113" t="s">
+      <c r="D3" s="115"/>
+      <c r="E3" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="113" t="s">
+      <c r="F3" s="115"/>
+      <c r="G3" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="114"/>
+      <c r="H3" s="115"/>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="30" t="s">
         <v>70</v>
       </c>
@@ -15086,23 +15086,23 @@
       <c r="H61" s="112"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="117" t="s">
+      <c r="A62" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="117"/>
-      <c r="C62" s="117">
+      <c r="B62" s="113"/>
+      <c r="C62" s="113">
         <f>C12+C19+C61+C40+C47+C54+C26+C33</f>
         <v>0</v>
       </c>
-      <c r="D62" s="117">
+      <c r="D62" s="113">
         <f>D12+D19+D61+D40+D47+D54+D26+D33</f>
         <v>0</v>
       </c>
-      <c r="E62" s="117">
+      <c r="E62" s="113">
         <f>E12+E19+E61+E40+E47+E54+E26+E33</f>
         <v>0</v>
       </c>
-      <c r="F62" s="117">
+      <c r="F62" s="113">
         <f>F12+F19+F61+F40+F47+F54+F26+F33</f>
         <v>0</v>
       </c>
@@ -15116,12 +15116,12 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="117"/>
-      <c r="B63" s="117"/>
-      <c r="C63" s="117"/>
-      <c r="D63" s="117"/>
-      <c r="E63" s="117"/>
-      <c r="F63" s="117"/>
+      <c r="A63" s="113"/>
+      <c r="B63" s="113"/>
+      <c r="C63" s="113"/>
+      <c r="D63" s="113"/>
+      <c r="E63" s="113"/>
+      <c r="F63" s="113"/>
       <c r="G63" s="110">
         <f>G62+H62</f>
         <v>0</v>
@@ -15130,25 +15130,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="G3:H3"/>
@@ -15165,6 +15146,25 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A20:H20"/>
     <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G40:H40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
@@ -15258,10 +15258,10 @@
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="36">
         <f>SUM(C5:C6)</f>
         <v>0</v>

</xml_diff>